<commit_message>
feat: Add hardcoded resume link and default message for LinkedIn outreach
</commit_message>
<xml_diff>
--- a/inb/linkedin-data.xlsx
+++ b/inb/linkedin-data.xlsx
@@ -846,8 +846,16 @@
           <t>CoinSwitch</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>no_connect_button</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">

</xml_diff>